<commit_message>
finishing everything except 3d
</commit_message>
<xml_diff>
--- a/xl_files/Q2d_results_Thor ragnarok_.xlsx
+++ b/xl_files/Q2d_results_Thor ragnarok_.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,82 +519,328 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>[('THOR', 0.6445623342175066), ('LOKI', 0.5348495964783566), ('HELA', 0.5237068965517241), ('SKURGE', 0.48342175066313)]</t>
+          <t>('THOR', 0.6445623342175066)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[('THOR', 37.58620689655172), ('HULK', 10.551724137931034), ('GRANDMASTER', 9.0), ('LOKI', 8.275862068965518)]</t>
+          <t>('THOR', 37.58620689655172)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[('THOR', 0.24314416822800877), ('HELA', 0.07312503340779225), ('GRANDMASTER', 0.06898321219232094), ('HULK', 0.06574365835938863)]</t>
+          <t>('THOR', 0.24314416822800877)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[('THOR', 0.7509578544061303), ('HELA', 0.6144200626959248), ('LOKI', 0.5752017608217168), ('VALKYRIE', 0.5752017608217168)]</t>
+          <t>('THOR', 0.7509578544061303)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[('THOR', 37.58620689655172), ('HULK', 10.551724137931034), ('GRANDMASTER', 9.0), ('LOKI', 8.275862068965518)]</t>
+          <t>('THOR', 37.58620689655172)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[('THOR', 0.2647385847069541), ('HULK', 0.0774216851848003), ('HELA', 0.0667386522665831), ('VALKYRIE', 0.0640080667296564)]</t>
+          <t>('THOR', 0.2647385847069541)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[('THOR', 0.6445623342175066), ('LOKI', 0.5348495964783566), ('HELA', 0.5237068965517241), ('SKURGE', 0.48342175066313)]</t>
+          <t>('THOR', 0.6445623342175066)</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[('THOR', 1.3103448275862069), ('HELA', 0.8275862068965517), ('VALKYRIE', 0.7586206896551724), ('LOKI', 0.7241379310344828)]</t>
+          <t>('THOR', 1.3103448275862069)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>[('THOR', 0.11601006274772567), ('ACTOR ODIN', 0.07640625846765385), ('HELA', 0.06760903388493916), ('LOKI', 0.06447003071072661)]</t>
+          <t>('THOR', 0.11601006274772567)</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>[('THOR', 0.45043103448275856), ('HELA', 0.1783456486042693), ('ODIN', 0.145935960591133), ('ACTOR THOR', 0.1268472906403941)]</t>
+          <t>('THOR', 0.45043103448275856)</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>[('THOR', 0.4587763990132245), ('LOKI', 0.3688008486065598), ('HELA', 0.3373091728863472), ('VALKYRIE', 0.3292933313556576)]</t>
+          <t>('THOR', 0.4587763990132245)</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[('THOR', 0.7509578544061303), ('HELA', 0.6144200626959248), ('LOKI', 0.5752017608217168), ('VALKYRIE', 0.5752017608217168)]</t>
+          <t>('THOR', 0.7509578544061303)</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>[('THOR', 0.7931034482758621), ('HELA', 0.5517241379310345), ('VALKYRIE', 0.5172413793103449), ('LOKI', 0.4482758620689655)]</t>
+          <t>('THOR', 0.7931034482758621)</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>[('THOR', 0.11833298461441616), ('HELA', 0.07943970345877638), ('VALKYRIE', 0.07188073664367498), ('LOKI', 0.06212328826857346)]</t>
+          <t>('THOR', 0.11833298461441616)</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>[('THOR', 0.4506568144499178), ('HELA', 0.15459770114942528), ('ODIN', 0.09967159277504102), ('VALKYRIE', 0.09478653530377669)]</t>
+          <t>('THOR', 0.4506568144499178)</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>[('THOR', 0.42757384785027275), ('HELA', 0.34805477659671785), ('VALKYRIE', 0.34525830280847697), ('LOKI', 0.32036312593878313)]</t>
+          <t>('THOR', 0.42757384785027275)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>('LOKI', 0.5348495964783566)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>('HULK', 10.551724137931034)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>('HELA', 0.07312503340779225)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>('HELA', 0.6144200626959248)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>('HULK', 10.551724137931034)</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>('HULK', 0.0774216851848003)</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>('LOKI', 0.5348495964783566)</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>('HELA', 0.8275862068965517)</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>('ACTOR ODIN', 0.07640625846765385)</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>('HELA', 0.1783456486042693)</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>('LOKI', 0.3688008486065598)</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>('HELA', 0.6144200626959248)</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>('HELA', 0.5517241379310345)</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>('HELA', 0.07943970345877638)</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>('HELA', 0.15459770114942528)</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>('HELA', 0.34805477659671785)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>('HELA', 0.5237068965517241)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>('GRANDMASTER', 9.0)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>('GRANDMASTER', 0.06898321219232094)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>('LOKI', 0.5752017608217168)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>('GRANDMASTER', 9.0)</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>('HELA', 0.0667386522665831)</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>('HELA', 0.5237068965517241)</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>('VALKYRIE', 0.7586206896551724)</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>('HELA', 0.06760903388493916)</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>('ODIN', 0.145935960591133)</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>('HELA', 0.3373091728863472)</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>('LOKI', 0.5752017608217168)</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>('VALKYRIE', 0.5172413793103449)</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>('VALKYRIE', 0.07188073664367498)</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>('ODIN', 0.09967159277504102)</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>('VALKYRIE', 0.34525830280847697)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>('SKURGE', 0.48342175066313)</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>('LOKI', 8.275862068965518)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>('HULK', 0.06574365835938863)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>('VALKYRIE', 0.5752017608217168)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>('LOKI', 8.275862068965518)</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>('VALKYRIE', 0.0640080667296564)</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>('SKURGE', 0.48342175066313)</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>('LOKI', 0.7241379310344828)</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>('LOKI', 0.06447003071072661)</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>('ACTOR THOR', 0.1268472906403941)</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>('VALKYRIE', 0.3292933313556576)</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>('VALKYRIE', 0.5752017608217168)</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>('LOKI', 0.4482758620689655)</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>('LOKI', 0.06212328826857346)</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>('VALKYRIE', 0.09478653530377669)</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>('LOKI', 0.32036312593878313)</t>
         </is>
       </c>
     </row>

</xml_diff>